<commit_message>
working on ga report
</commit_message>
<xml_diff>
--- a/public/download/sample/Rso List.xlsx
+++ b/public/download/sample/Rso List.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12375"/>
+    <workbookView windowWidth="28800" windowHeight="12315"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -430,346 +430,346 @@
     <t>0000000007</t>
   </si>
   <si>
+    <t>MYMVAI01_ROUTE05,MYMVAI01_ROUTE06</t>
+  </si>
+  <si>
+    <t>RS008290</t>
+  </si>
+  <si>
+    <t>01986646474</t>
+  </si>
+  <si>
+    <t>01935592053</t>
+  </si>
+  <si>
+    <t>01983342880</t>
+  </si>
+  <si>
+    <t>RGAZ0049</t>
+  </si>
+  <si>
+    <t>SR-09</t>
+  </si>
+  <si>
+    <t>Anwar Uddin</t>
+  </si>
+  <si>
+    <t>Shamima Akter</t>
+  </si>
+  <si>
+    <t>Chaysuti, Kuliarchar, Kishoreganj.</t>
+  </si>
+  <si>
+    <t>173.103.0011174</t>
+  </si>
+  <si>
+    <t>0000000008</t>
+  </si>
+  <si>
+    <t>MYMVAI01_ROUTE24,MYMVAI01_ROUTE25</t>
+  </si>
+  <si>
+    <t>RS010508</t>
+  </si>
+  <si>
+    <t>01986686880</t>
+  </si>
+  <si>
+    <t>01935591915</t>
+  </si>
+  <si>
+    <t>01924303333</t>
+  </si>
+  <si>
+    <t>RGAZ0379</t>
+  </si>
+  <si>
+    <t>SR-13</t>
+  </si>
+  <si>
+    <t>Md. Harich Mia</t>
+  </si>
+  <si>
+    <t>Jahanara Begum</t>
+  </si>
+  <si>
+    <t>Akbornagar, 2350, Bhairab, Kishoreganj.</t>
+  </si>
+  <si>
+    <t>173.103.0011127</t>
+  </si>
+  <si>
+    <t>0000000009</t>
+  </si>
+  <si>
+    <t>MYMVAI02</t>
+  </si>
+  <si>
+    <t>01923909897</t>
+  </si>
+  <si>
+    <t>MYMVAI02_ROUTE0001,MYMVAI02_ROUTE0002</t>
+  </si>
+  <si>
+    <t>RS035430</t>
+  </si>
+  <si>
+    <t>01409944002</t>
+  </si>
+  <si>
+    <t>01935593313</t>
+  </si>
+  <si>
+    <t>01912431177</t>
+  </si>
+  <si>
+    <t>RGAZ0178</t>
+  </si>
+  <si>
+    <t>SR-26</t>
+  </si>
+  <si>
+    <t>Md. Soleman</t>
+  </si>
+  <si>
+    <t>Minara Khatun</t>
+  </si>
+  <si>
+    <t>Savianagar, Astagram, Kishoreganj.</t>
+  </si>
+  <si>
+    <t>173.151.0221312</t>
+  </si>
+  <si>
+    <t>0000000010</t>
+  </si>
+  <si>
+    <t>MYMVAI02_ROUTE0003,MYMVAI02_ROUTE0003</t>
+  </si>
+  <si>
+    <t>RS035431</t>
+  </si>
+  <si>
+    <t>01915270104</t>
+  </si>
+  <si>
+    <t>01935591816</t>
+  </si>
+  <si>
+    <t>01992501390</t>
+  </si>
+  <si>
+    <t>RGAZ0337</t>
+  </si>
+  <si>
+    <t>SR-04</t>
+  </si>
+  <si>
+    <t>Md. Korim</t>
+  </si>
+  <si>
+    <t>Shahanaj</t>
+  </si>
+  <si>
+    <t>Baniya Hati, Itna, Kishoreganj.</t>
+  </si>
+  <si>
+    <t>AB+</t>
+  </si>
+  <si>
+    <t>231.158.0071652</t>
+  </si>
+  <si>
+    <t>0000000011</t>
+  </si>
+  <si>
+    <t>MYMVAI02_ROUTE0005,MYMVAI02_ROUTE0006</t>
+  </si>
+  <si>
+    <t>RS035432</t>
+  </si>
+  <si>
+    <t>01915270105</t>
+  </si>
+  <si>
+    <t>01935591916</t>
+  </si>
+  <si>
+    <t>01312914994</t>
+  </si>
+  <si>
+    <t>RGAZ0338</t>
+  </si>
+  <si>
+    <t>SR-05</t>
+  </si>
+  <si>
+    <t>Siddikur Rahman</t>
+  </si>
+  <si>
+    <t>Roshena Akter</t>
+  </si>
+  <si>
+    <t>Vati Ghagra, Mithamoin, Kishoreganj.</t>
+  </si>
+  <si>
+    <t>A+</t>
+  </si>
+  <si>
+    <t>231.158.0071374</t>
+  </si>
+  <si>
+    <t>0000000012</t>
+  </si>
+  <si>
+    <t>MYMVAI02_ROUTE0007,MYMVAI02_ROUTE0008</t>
+  </si>
+  <si>
+    <t>RS035433</t>
+  </si>
+  <si>
+    <t>01967042950</t>
+  </si>
+  <si>
+    <t>01935592484</t>
+  </si>
+  <si>
+    <t>01304255571</t>
+  </si>
+  <si>
+    <t>RGAZ0258</t>
+  </si>
+  <si>
+    <t>SR-24</t>
+  </si>
+  <si>
+    <t>Md. Mostofa Hossein</t>
+  </si>
+  <si>
+    <t>Josna Begum</t>
+  </si>
+  <si>
+    <t>Sihara, Vati Ghagra, Mithamoin, Kishoreganj.</t>
+  </si>
+  <si>
+    <t>173.158.0022692</t>
+  </si>
+  <si>
+    <t>0000000013</t>
+  </si>
+  <si>
+    <t>MYMVAI02_ROUTE0009,MYMVAI02_ROUTE0010</t>
+  </si>
+  <si>
+    <t>RS035434</t>
+  </si>
+  <si>
+    <t>01986686877</t>
+  </si>
+  <si>
+    <t>01935591836</t>
+  </si>
+  <si>
+    <t>01309213222</t>
+  </si>
+  <si>
+    <t>RGAZ0339</t>
+  </si>
+  <si>
+    <t>SR-10</t>
+  </si>
+  <si>
+    <t>Ab. Sattar Mia</t>
+  </si>
+  <si>
+    <t>Mst. Mirjan</t>
+  </si>
+  <si>
+    <t>Darikapur, Itna, Kishoreganj.</t>
+  </si>
+  <si>
+    <t>231.103.0044922</t>
+  </si>
+  <si>
+    <t>0000000014</t>
+  </si>
+  <si>
+    <t>MYMVAI02_ROUTE0011,MYMVAI02_ROUTE0012</t>
+  </si>
+  <si>
+    <t>RS035435</t>
+  </si>
+  <si>
+    <t>01986686878</t>
+  </si>
+  <si>
+    <t>01935591828</t>
+  </si>
+  <si>
+    <t>01905308282</t>
+  </si>
+  <si>
+    <t>RGAZ0018</t>
+  </si>
+  <si>
+    <t>SR-11</t>
+  </si>
+  <si>
+    <t>Ali Islam</t>
+  </si>
+  <si>
+    <t>Nasima Akter</t>
+  </si>
+  <si>
+    <t>Purbo astagram, Astagram, Kishoreganj.</t>
+  </si>
+  <si>
+    <t>173.103.0011244</t>
+  </si>
+  <si>
+    <t>0000000015</t>
+  </si>
+  <si>
+    <t>MYMVAI02_ROUTE0013,MYMVAI02_ROUTE0014</t>
+  </si>
+  <si>
+    <t>RS035436</t>
+  </si>
+  <si>
+    <t>01986686879</t>
+  </si>
+  <si>
+    <t>01935592119</t>
+  </si>
+  <si>
+    <t>01608613676</t>
+  </si>
+  <si>
+    <t>RGAZ0260</t>
+  </si>
+  <si>
+    <t>SR-12</t>
+  </si>
+  <si>
+    <t>Md. Ashrab Ali</t>
+  </si>
+  <si>
+    <t>Mst. Khodeja Begum</t>
+  </si>
+  <si>
+    <t>Katkhal, Mithamoin, Kishoreganj.</t>
+  </si>
+  <si>
+    <t>173.158.23091</t>
+  </si>
+  <si>
+    <t>0000000016</t>
+  </si>
+  <si>
+    <t>MYMVAI03</t>
+  </si>
+  <si>
     <t>01923909899</t>
-  </si>
-  <si>
-    <t>MYMVAI01_ROUTE05,MYMVAI01_ROUTE06</t>
-  </si>
-  <si>
-    <t>RS008290</t>
-  </si>
-  <si>
-    <t>01986646474</t>
-  </si>
-  <si>
-    <t>01935592053</t>
-  </si>
-  <si>
-    <t>01983342880</t>
-  </si>
-  <si>
-    <t>RGAZ0049</t>
-  </si>
-  <si>
-    <t>SR-09</t>
-  </si>
-  <si>
-    <t>Anwar Uddin</t>
-  </si>
-  <si>
-    <t>Shamima Akter</t>
-  </si>
-  <si>
-    <t>Chaysuti, Kuliarchar, Kishoreganj.</t>
-  </si>
-  <si>
-    <t>173.103.0011174</t>
-  </si>
-  <si>
-    <t>0000000008</t>
-  </si>
-  <si>
-    <t>MYMVAI01_ROUTE24,MYMVAI01_ROUTE25</t>
-  </si>
-  <si>
-    <t>RS010508</t>
-  </si>
-  <si>
-    <t>01986686880</t>
-  </si>
-  <si>
-    <t>01935591915</t>
-  </si>
-  <si>
-    <t>01924303333</t>
-  </si>
-  <si>
-    <t>RGAZ0379</t>
-  </si>
-  <si>
-    <t>SR-13</t>
-  </si>
-  <si>
-    <t>Md. Harich Mia</t>
-  </si>
-  <si>
-    <t>Jahanara Begum</t>
-  </si>
-  <si>
-    <t>Akbornagar, 2350, Bhairab, Kishoreganj.</t>
-  </si>
-  <si>
-    <t>173.103.0011127</t>
-  </si>
-  <si>
-    <t>0000000009</t>
-  </si>
-  <si>
-    <t>MYMVAI02</t>
-  </si>
-  <si>
-    <t>01923909897</t>
-  </si>
-  <si>
-    <t>MYMVAI02_ROUTE0001,MYMVAI02_ROUTE0002</t>
-  </si>
-  <si>
-    <t>RS035430</t>
-  </si>
-  <si>
-    <t>01409944002</t>
-  </si>
-  <si>
-    <t>01935593313</t>
-  </si>
-  <si>
-    <t>01912431177</t>
-  </si>
-  <si>
-    <t>RGAZ0178</t>
-  </si>
-  <si>
-    <t>SR-26</t>
-  </si>
-  <si>
-    <t>Md. Soleman</t>
-  </si>
-  <si>
-    <t>Minara Khatun</t>
-  </si>
-  <si>
-    <t>Savianagar, Astagram, Kishoreganj.</t>
-  </si>
-  <si>
-    <t>173.151.0221312</t>
-  </si>
-  <si>
-    <t>0000000010</t>
-  </si>
-  <si>
-    <t>MYMVAI02_ROUTE0003,MYMVAI02_ROUTE0003</t>
-  </si>
-  <si>
-    <t>RS035431</t>
-  </si>
-  <si>
-    <t>01915270104</t>
-  </si>
-  <si>
-    <t>01935591816</t>
-  </si>
-  <si>
-    <t>01992501390</t>
-  </si>
-  <si>
-    <t>RGAZ0337</t>
-  </si>
-  <si>
-    <t>SR-04</t>
-  </si>
-  <si>
-    <t>Md. Korim</t>
-  </si>
-  <si>
-    <t>Shahanaj</t>
-  </si>
-  <si>
-    <t>Baniya Hati, Itna, Kishoreganj.</t>
-  </si>
-  <si>
-    <t>AB+</t>
-  </si>
-  <si>
-    <t>231.158.0071652</t>
-  </si>
-  <si>
-    <t>0000000011</t>
-  </si>
-  <si>
-    <t>MYMVAI02_ROUTE0005,MYMVAI02_ROUTE0006</t>
-  </si>
-  <si>
-    <t>RS035432</t>
-  </si>
-  <si>
-    <t>01915270105</t>
-  </si>
-  <si>
-    <t>01935591916</t>
-  </si>
-  <si>
-    <t>01312914994</t>
-  </si>
-  <si>
-    <t>RGAZ0338</t>
-  </si>
-  <si>
-    <t>SR-05</t>
-  </si>
-  <si>
-    <t>Siddikur Rahman</t>
-  </si>
-  <si>
-    <t>Roshena Akter</t>
-  </si>
-  <si>
-    <t>Vati Ghagra, Mithamoin, Kishoreganj.</t>
-  </si>
-  <si>
-    <t>A+</t>
-  </si>
-  <si>
-    <t>231.158.0071374</t>
-  </si>
-  <si>
-    <t>0000000012</t>
-  </si>
-  <si>
-    <t>MYMVAI02_ROUTE0007,MYMVAI02_ROUTE0008</t>
-  </si>
-  <si>
-    <t>RS035433</t>
-  </si>
-  <si>
-    <t>01967042950</t>
-  </si>
-  <si>
-    <t>01935592484</t>
-  </si>
-  <si>
-    <t>01304255571</t>
-  </si>
-  <si>
-    <t>RGAZ0258</t>
-  </si>
-  <si>
-    <t>SR-24</t>
-  </si>
-  <si>
-    <t>Md. Mostofa Hossein</t>
-  </si>
-  <si>
-    <t>Josna Begum</t>
-  </si>
-  <si>
-    <t>Sihara, Vati Ghagra, Mithamoin, Kishoreganj.</t>
-  </si>
-  <si>
-    <t>173.158.0022692</t>
-  </si>
-  <si>
-    <t>0000000013</t>
-  </si>
-  <si>
-    <t>MYMVAI02_ROUTE0009,MYMVAI02_ROUTE0010</t>
-  </si>
-  <si>
-    <t>RS035434</t>
-  </si>
-  <si>
-    <t>01986686877</t>
-  </si>
-  <si>
-    <t>01935591836</t>
-  </si>
-  <si>
-    <t>01309213222</t>
-  </si>
-  <si>
-    <t>RGAZ0339</t>
-  </si>
-  <si>
-    <t>SR-10</t>
-  </si>
-  <si>
-    <t>Ab. Sattar Mia</t>
-  </si>
-  <si>
-    <t>Mst. Mirjan</t>
-  </si>
-  <si>
-    <t>Darikapur, Itna, Kishoreganj.</t>
-  </si>
-  <si>
-    <t>231.103.0044922</t>
-  </si>
-  <si>
-    <t>0000000014</t>
-  </si>
-  <si>
-    <t>MYMVAI02_ROUTE0011,MYMVAI02_ROUTE0012</t>
-  </si>
-  <si>
-    <t>RS035435</t>
-  </si>
-  <si>
-    <t>01986686878</t>
-  </si>
-  <si>
-    <t>01935591828</t>
-  </si>
-  <si>
-    <t>01905308282</t>
-  </si>
-  <si>
-    <t>RGAZ0018</t>
-  </si>
-  <si>
-    <t>SR-11</t>
-  </si>
-  <si>
-    <t>Ali Islam</t>
-  </si>
-  <si>
-    <t>Nasima Akter</t>
-  </si>
-  <si>
-    <t>Purbo astagram, Astagram, Kishoreganj.</t>
-  </si>
-  <si>
-    <t>173.103.0011244</t>
-  </si>
-  <si>
-    <t>0000000015</t>
-  </si>
-  <si>
-    <t>MYMVAI02_ROUTE0013,MYMVAI02_ROUTE0014</t>
-  </si>
-  <si>
-    <t>RS035436</t>
-  </si>
-  <si>
-    <t>01986686879</t>
-  </si>
-  <si>
-    <t>01935592119</t>
-  </si>
-  <si>
-    <t>01608613676</t>
-  </si>
-  <si>
-    <t>RGAZ0260</t>
-  </si>
-  <si>
-    <t>SR-12</t>
-  </si>
-  <si>
-    <t>Md. Ashrab Ali</t>
-  </si>
-  <si>
-    <t>Mst. Khodeja Begum</t>
-  </si>
-  <si>
-    <t>Katkhal, Mithamoin, Kishoreganj.</t>
-  </si>
-  <si>
-    <t>173.158.23091</t>
-  </si>
-  <si>
-    <t>0000000016</t>
-  </si>
-  <si>
-    <t>MYMVAI03</t>
   </si>
   <si>
     <t>MYMVAI03_ROUTE0001,MYMVAI03_ROUTE0002</t>
@@ -1110,17 +1110,32 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="0_);[Red]\(0\)"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="[$-409]d/mmm/yyyy;@"/>
-    <numFmt numFmtId="179" formatCode="0_);[Red]\(0\)"/>
+    <numFmt numFmtId="179" formatCode="[$-409]d/mmm/yyyy;@"/>
   </numFmts>
   <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1133,9 +1148,37 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1158,22 +1201,51 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1187,45 +1259,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1238,42 +1274,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -1284,7 +1284,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1296,7 +1308,121 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1308,55 +1434,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1368,103 +1458,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1475,6 +1475,30 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1498,36 +1522,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -1537,11 +1531,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1561,16 +1561,16 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
+      <right style="double">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
+      <top style="double">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
+      <bottom style="double">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -1580,15 +1580,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -1598,131 +1598,131 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1736,10 +1736,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2071,7 +2071,7 @@
   <dimension ref="A1:AC27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -2894,34 +2894,34 @@
         <v>28</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="H10" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="I10" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="I10" s="1" t="s">
+      <c r="J10" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="J10" s="1" t="s">
+      <c r="K10" s="1" t="s">
         <v>146</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>147</v>
       </c>
       <c r="L10" s="1" t="s">
         <v>39</v>
@@ -2933,13 +2933,13 @@
         <v>41</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="P10" s="1" t="s">
         <v>43</v>
       </c>
       <c r="Q10" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="R10" s="1" t="s">
         <v>45</v>
@@ -2948,7 +2948,7 @@
         <v>18</v>
       </c>
       <c r="T10" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="U10" s="1">
         <v>8250</v>
@@ -2984,31 +2984,31 @@
         <v>29</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="G11" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="H11" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="I11" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="J11" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="J11" s="1" t="s">
+      <c r="K11" s="1" t="s">
         <v>158</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>159</v>
       </c>
       <c r="L11" s="1" t="s">
         <v>39</v>
@@ -3020,13 +3020,13 @@
         <v>41</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="P11" s="1" t="s">
         <v>73</v>
       </c>
       <c r="Q11" s="6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="R11" s="1" t="s">
         <v>45</v>
@@ -3035,7 +3035,7 @@
         <v>18</v>
       </c>
       <c r="T11" s="6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="U11" s="1">
         <v>7000</v>
@@ -3065,37 +3065,37 @@
     </row>
     <row r="12" spans="1:29">
       <c r="A12" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="G12" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="H12" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="I12" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="I12" s="1" t="s">
+      <c r="J12" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="J12" s="1" t="s">
+      <c r="K12" s="1" t="s">
         <v>172</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>173</v>
       </c>
       <c r="L12" s="1" t="s">
         <v>39</v>
@@ -3107,13 +3107,13 @@
         <v>41</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="P12" s="1" t="s">
         <v>73</v>
       </c>
       <c r="Q12" s="6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="R12" s="1" t="s">
         <v>45</v>
@@ -3122,7 +3122,7 @@
         <v>18</v>
       </c>
       <c r="T12" s="6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="U12" s="1">
         <v>7000</v>
@@ -3152,37 +3152,37 @@
     </row>
     <row r="13" spans="1:29">
       <c r="A13" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>164</v>
-      </c>
       <c r="C13" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="G13" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="H13" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="I13" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="I13" s="1" t="s">
+      <c r="J13" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="J13" s="1" t="s">
+      <c r="K13" s="1" t="s">
         <v>184</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>185</v>
       </c>
       <c r="L13" s="1" t="s">
         <v>39</v>
@@ -3194,13 +3194,13 @@
         <v>41</v>
       </c>
       <c r="O13" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="P13" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="P13" s="1" t="s">
+      <c r="Q13" s="6" t="s">
         <v>187</v>
-      </c>
-      <c r="Q13" s="6" t="s">
-        <v>188</v>
       </c>
       <c r="R13" s="1" t="s">
         <v>45</v>
@@ -3209,7 +3209,7 @@
         <v>18</v>
       </c>
       <c r="T13" s="6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="U13" s="1">
         <v>7000</v>
@@ -3239,37 +3239,37 @@
     </row>
     <row r="14" spans="1:29">
       <c r="A14" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>164</v>
-      </c>
       <c r="C14" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="G14" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="H14" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="H14" s="1" t="s">
+      <c r="I14" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="I14" s="1" t="s">
+      <c r="J14" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="J14" s="1" t="s">
+      <c r="K14" s="1" t="s">
         <v>197</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>198</v>
       </c>
       <c r="L14" s="1" t="s">
         <v>39</v>
@@ -3281,13 +3281,13 @@
         <v>41</v>
       </c>
       <c r="O14" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="P14" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="P14" s="1" t="s">
+      <c r="Q14" s="6" t="s">
         <v>200</v>
-      </c>
-      <c r="Q14" s="6" t="s">
-        <v>201</v>
       </c>
       <c r="R14" s="1" t="s">
         <v>45</v>
@@ -3296,7 +3296,7 @@
         <v>18</v>
       </c>
       <c r="T14" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="U14" s="1">
         <v>7000</v>
@@ -3326,37 +3326,37 @@
     </row>
     <row r="15" spans="1:29">
       <c r="A15" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>164</v>
-      </c>
       <c r="C15" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="F15" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="G15" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="H15" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="H15" s="1" t="s">
+      <c r="I15" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="I15" s="1" t="s">
+      <c r="J15" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="J15" s="1" t="s">
+      <c r="K15" s="1" t="s">
         <v>210</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>211</v>
       </c>
       <c r="L15" s="1" t="s">
         <v>39</v>
@@ -3368,13 +3368,13 @@
         <v>41</v>
       </c>
       <c r="O15" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="P15" s="1" t="s">
         <v>73</v>
       </c>
       <c r="Q15" s="6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="R15" s="1" t="s">
         <v>45</v>
@@ -3383,7 +3383,7 @@
         <v>18</v>
       </c>
       <c r="T15" s="6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="U15" s="1">
         <v>7000</v>
@@ -3413,37 +3413,37 @@
     </row>
     <row r="16" spans="1:29">
       <c r="A16" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>164</v>
-      </c>
       <c r="C16" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="F16" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="G16" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="H16" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="H16" s="1" t="s">
+      <c r="I16" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="I16" s="1" t="s">
+      <c r="J16" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="J16" s="1" t="s">
+      <c r="K16" s="1" t="s">
         <v>222</v>
-      </c>
-      <c r="K16" s="1" t="s">
-        <v>223</v>
       </c>
       <c r="L16" s="1" t="s">
         <v>39</v>
@@ -3455,13 +3455,13 @@
         <v>41</v>
       </c>
       <c r="O16" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="P16" s="1" t="s">
         <v>43</v>
       </c>
       <c r="Q16" s="6" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="R16" s="1" t="s">
         <v>45</v>
@@ -3470,7 +3470,7 @@
         <v>18</v>
       </c>
       <c r="T16" s="6" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="U16" s="1">
         <v>7000</v>
@@ -3500,37 +3500,37 @@
     </row>
     <row r="17" spans="1:29">
       <c r="A17" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>164</v>
-      </c>
       <c r="C17" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="F17" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="G17" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="H17" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="I17" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="I17" s="1" t="s">
+      <c r="J17" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="J17" s="1" t="s">
+      <c r="K17" s="1" t="s">
         <v>234</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>235</v>
       </c>
       <c r="L17" s="1" t="s">
         <v>39</v>
@@ -3542,13 +3542,13 @@
         <v>41</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="P17" s="1" t="s">
         <v>73</v>
       </c>
       <c r="Q17" s="6" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="R17" s="1" t="s">
         <v>45</v>
@@ -3557,7 +3557,7 @@
         <v>18</v>
       </c>
       <c r="T17" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="U17" s="1">
         <v>7000</v>
@@ -3587,37 +3587,37 @@
     </row>
     <row r="18" spans="1:29">
       <c r="A18" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>164</v>
-      </c>
       <c r="C18" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="F18" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="G18" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="G18" s="1" t="s">
+      <c r="H18" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="H18" s="1" t="s">
+      <c r="I18" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="I18" s="1" t="s">
+      <c r="J18" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="J18" s="1" t="s">
+      <c r="K18" s="1" t="s">
         <v>246</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>247</v>
       </c>
       <c r="L18" s="1" t="s">
         <v>39</v>
@@ -3629,13 +3629,13 @@
         <v>41</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="P18" s="1" t="s">
         <v>43</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="R18" s="1" t="s">
         <v>45</v>
@@ -3644,7 +3644,7 @@
         <v>18</v>
       </c>
       <c r="T18" s="6" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="U18" s="1">
         <v>7000</v>
@@ -3674,10 +3674,10 @@
     </row>
     <row r="19" spans="1:29">
       <c r="A19" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>251</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>138</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>252</v>
@@ -3761,10 +3761,10 @@
     </row>
     <row r="20" spans="1:29">
       <c r="A20" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>251</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>138</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>265</v>
@@ -3806,7 +3806,7 @@
         <v>274</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="Q20" s="6" t="s">
         <v>275</v>
@@ -3848,10 +3848,10 @@
     </row>
     <row r="21" spans="1:29">
       <c r="A21" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>251</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>138</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>277</v>
@@ -3935,10 +3935,10 @@
     </row>
     <row r="22" spans="1:29">
       <c r="A22" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>251</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>164</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>289</v>
@@ -4022,10 +4022,10 @@
     </row>
     <row r="23" spans="1:29">
       <c r="A23" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>251</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>138</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>301</v>
@@ -4109,10 +4109,10 @@
     </row>
     <row r="24" spans="1:29">
       <c r="A24" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>251</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>138</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>312</v>
@@ -4196,10 +4196,10 @@
     </row>
     <row r="25" spans="1:29">
       <c r="A25" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>251</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>138</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>325</v>
@@ -4283,10 +4283,10 @@
     </row>
     <row r="26" spans="1:29">
       <c r="A26" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>251</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>138</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>337</v>
@@ -4370,10 +4370,10 @@
     </row>
     <row r="27" spans="1:29">
       <c r="A27" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>251</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>138</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>349</v>

</xml_diff>

<commit_message>
Remove ajax insert and update
</commit_message>
<xml_diff>
--- a/public/download/sample/Rso List.xlsx
+++ b/public/download/sample/Rso List.xlsx
@@ -1,34 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Installed Software\xampp\htdocs\enstudio\public\download\sample\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71CAECED-2CCB-4304-8598-4E93A2043857}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="28800" windowHeight="12210"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="653" uniqueCount="363">
   <si>
     <t>DD Code</t>
   </si>
@@ -1117,53 +1103,21 @@
   </si>
   <si>
     <t>5123019746</t>
-  </si>
-  <si>
-    <t>RS000000</t>
-  </si>
-  <si>
-    <t>01908441957</t>
-  </si>
-  <si>
-    <t>SR-00</t>
-  </si>
-  <si>
-    <t>MYMVAI02_ROUTE0004</t>
-  </si>
-  <si>
-    <t>01935000000</t>
-  </si>
-  <si>
-    <t>01911000000</t>
-  </si>
-  <si>
-    <t>RGAZ0001</t>
-  </si>
-  <si>
-    <t>মমতাজ উদ্দিন</t>
-  </si>
-  <si>
-    <t>সুরাইয়া বেগম</t>
-  </si>
-  <si>
-    <t>Cupidatat sunt neces</t>
-  </si>
-  <si>
-    <t>1730000000000</t>
-  </si>
-  <si>
-    <t>0000000026</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="0_);[Red]\(0\)"/>
-    <numFmt numFmtId="167" formatCode="[$-409]d/mmm/yyyy;@"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
+  <numFmts count="6">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="[$-409]d/mmm/yyyy;@"/>
+    <numFmt numFmtId="179" formatCode="0_);[Red]\(0\)"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1172,26 +1126,350 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <charset val="134"/>
     </font>
-    <font>
-      <sz val="8"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -1199,54 +1477,337 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" quotePrefix="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="50">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
+    <cellStyle name="Output" xfId="17" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Good" xfId="22" builtinId="26"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
+    <cellStyle name="Normal 2" xfId="49"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1504,53 +2065,52 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AC31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:AC30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AB28" sqref="AB28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="45.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" style="7" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="6.42578125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="22.140625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="24.42578125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="8.7109375" style="1" customWidth="1"/>
-    <col min="13" max="13" width="12.28515625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="12.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="11.2857142857143" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.8571428571429" style="1" customWidth="1"/>
+    <col min="3" max="3" width="45.2857142857143" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.71428571428571" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.1428571428571" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7142857142857" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.8571428571429" style="2" customWidth="1"/>
+    <col min="8" max="8" width="10.2857142857143" style="1" customWidth="1"/>
+    <col min="9" max="9" width="6.42857142857143" style="1" customWidth="1"/>
+    <col min="10" max="10" width="22.1428571428571" style="1" customWidth="1"/>
+    <col min="11" max="11" width="24.4285714285714" style="1" customWidth="1"/>
+    <col min="12" max="12" width="8.71428571428571" style="1" customWidth="1"/>
+    <col min="13" max="13" width="12.2857142857143" style="1" customWidth="1"/>
+    <col min="14" max="14" width="12.8571428571429" style="1" customWidth="1"/>
     <col min="15" max="15" width="63" style="1" customWidth="1"/>
-    <col min="16" max="16" width="12.85546875" style="1" customWidth="1"/>
-    <col min="17" max="17" width="17.28515625" style="1" customWidth="1"/>
-    <col min="18" max="18" width="11.85546875" style="1" customWidth="1"/>
-    <col min="19" max="19" width="13.85546875" style="1" customWidth="1"/>
-    <col min="20" max="20" width="16.85546875" style="1" customWidth="1"/>
-    <col min="21" max="21" width="6.85546875" style="1" customWidth="1"/>
-    <col min="22" max="22" width="10.28515625" style="1" customWidth="1"/>
-    <col min="23" max="23" width="14.140625" style="1" customWidth="1"/>
-    <col min="24" max="24" width="8.140625" style="1" customWidth="1"/>
-    <col min="25" max="25" width="13.42578125" style="1" customWidth="1"/>
-    <col min="26" max="26" width="20.140625" style="1" customWidth="1"/>
-    <col min="27" max="27" width="15.7109375" style="1" customWidth="1"/>
-    <col min="28" max="28" width="12.7109375" style="1" customWidth="1"/>
-    <col min="29" max="16384" width="9.140625" style="1"/>
+    <col min="16" max="16" width="12.8571428571429" style="1" customWidth="1"/>
+    <col min="17" max="17" width="17.2857142857143" style="1" customWidth="1"/>
+    <col min="18" max="18" width="11.8571428571429" style="1" customWidth="1"/>
+    <col min="19" max="19" width="13.8571428571429" style="1" customWidth="1"/>
+    <col min="20" max="20" width="16.8571428571429" style="1" customWidth="1"/>
+    <col min="21" max="21" width="6.85714285714286" style="1" customWidth="1"/>
+    <col min="22" max="22" width="10.2857142857143" style="1" customWidth="1"/>
+    <col min="23" max="23" width="14.1428571428571" style="1" customWidth="1"/>
+    <col min="24" max="24" width="8.14285714285714" style="1" customWidth="1"/>
+    <col min="25" max="25" width="13.4285714285714" style="1" customWidth="1"/>
+    <col min="26" max="26" width="20.1428571428571" style="1" customWidth="1"/>
+    <col min="27" max="27" width="15.7142857142857" style="1" customWidth="1"/>
+    <col min="28" max="28" width="12.7142857142857" style="1" customWidth="1"/>
+    <col min="29" max="16384" width="9.14285714285714" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29">
+    <row r="1" spans="1:28">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1569,7 +2129,7 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
@@ -1655,7 +2215,7 @@
       <c r="F2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="2" t="s">
         <v>34</v>
       </c>
       <c r="H2" s="1" t="s">
@@ -1685,7 +2245,7 @@
       <c r="P2" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="Q2" s="6" t="s">
+      <c r="Q2" s="7" t="s">
         <v>44</v>
       </c>
       <c r="R2" s="1" t="s">
@@ -1694,7 +2254,7 @@
       <c r="S2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T2" s="6" t="s">
+      <c r="T2" s="7" t="s">
         <v>46</v>
       </c>
       <c r="U2" s="1">
@@ -1709,19 +2269,19 @@
       <c r="X2" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="Y2" s="3">
+      <c r="Y2" s="4">
         <v>36842</v>
       </c>
-      <c r="Z2" s="4">
+      <c r="Z2" s="5">
         <v>8712043201</v>
       </c>
       <c r="AA2" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AB2" s="3">
+      <c r="AB2" s="4">
         <v>44743</v>
       </c>
-      <c r="AC2" s="5"/>
+      <c r="AC2" s="6"/>
     </row>
     <row r="3" spans="1:29">
       <c r="A3" s="1" t="s">
@@ -1742,7 +2302,7 @@
       <c r="F3" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="2" t="s">
         <v>54</v>
       </c>
       <c r="H3" s="1" t="s">
@@ -1772,7 +2332,7 @@
       <c r="P3" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="Q3" s="6" t="s">
+      <c r="Q3" s="7" t="s">
         <v>60</v>
       </c>
       <c r="R3" s="1" t="s">
@@ -1781,7 +2341,7 @@
       <c r="S3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T3" s="6" t="s">
+      <c r="T3" s="7" t="s">
         <v>61</v>
       </c>
       <c r="U3" s="1">
@@ -1796,19 +2356,19 @@
       <c r="X3" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="Y3" s="3">
+      <c r="Y3" s="4">
         <v>29571</v>
       </c>
-      <c r="Z3" s="4">
+      <c r="Z3" s="5">
         <v>3617160000000</v>
       </c>
       <c r="AA3" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AB3" s="3">
+      <c r="AB3" s="4">
         <v>43160</v>
       </c>
-      <c r="AC3" s="5"/>
+      <c r="AC3" s="6"/>
     </row>
     <row r="4" spans="1:29">
       <c r="A4" s="1" t="s">
@@ -1829,7 +2389,7 @@
       <c r="F4" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="2" t="s">
         <v>67</v>
       </c>
       <c r="H4" s="1" t="s">
@@ -1859,7 +2419,7 @@
       <c r="P4" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="Q4" s="6" t="s">
+      <c r="Q4" s="7" t="s">
         <v>74</v>
       </c>
       <c r="R4" s="1" t="s">
@@ -1868,7 +2428,7 @@
       <c r="S4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T4" s="6" t="s">
+      <c r="T4" s="7" t="s">
         <v>75</v>
       </c>
       <c r="U4" s="1">
@@ -1883,19 +2443,19 @@
       <c r="X4" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="Y4" s="3">
+      <c r="Y4" s="4">
         <v>32774</v>
       </c>
-      <c r="Z4" s="4">
+      <c r="Z4" s="5">
         <v>5821408877400</v>
       </c>
       <c r="AA4" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AB4" s="3">
+      <c r="AB4" s="4">
         <v>44621</v>
       </c>
-      <c r="AC4" s="5"/>
+      <c r="AC4" s="6"/>
     </row>
     <row r="5" spans="1:29">
       <c r="A5" s="1" t="s">
@@ -1916,7 +2476,7 @@
       <c r="F5" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="2" t="s">
         <v>80</v>
       </c>
       <c r="H5" s="1" t="s">
@@ -1946,7 +2506,7 @@
       <c r="P5" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="Q5" s="6" t="s">
+      <c r="Q5" s="7" t="s">
         <v>87</v>
       </c>
       <c r="R5" s="1" t="s">
@@ -1955,7 +2515,7 @@
       <c r="S5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T5" s="6" t="s">
+      <c r="T5" s="7" t="s">
         <v>89</v>
       </c>
       <c r="U5" s="1">
@@ -1970,19 +2530,19 @@
       <c r="X5" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="Y5" s="3">
+      <c r="Y5" s="4">
         <v>37235</v>
       </c>
-      <c r="Z5" s="4">
+      <c r="Z5" s="5">
         <v>7811121008700</v>
       </c>
       <c r="AA5" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AB5" s="3">
+      <c r="AB5" s="4">
         <v>43525</v>
       </c>
-      <c r="AC5" s="5"/>
+      <c r="AC5" s="6"/>
     </row>
     <row r="6" spans="1:29">
       <c r="A6" s="1" t="s">
@@ -2003,7 +2563,7 @@
       <c r="F6" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="G6" s="2" t="s">
         <v>94</v>
       </c>
       <c r="H6" s="1" t="s">
@@ -2033,7 +2593,7 @@
       <c r="P6" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="Q6" s="6" t="s">
+      <c r="Q6" s="7" t="s">
         <v>100</v>
       </c>
       <c r="R6" s="1" t="s">
@@ -2042,7 +2602,7 @@
       <c r="S6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T6" s="6" t="s">
+      <c r="T6" s="7" t="s">
         <v>101</v>
       </c>
       <c r="U6" s="1">
@@ -2057,19 +2617,19 @@
       <c r="X6" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="Y6" s="3">
+      <c r="Y6" s="4">
         <v>32874</v>
       </c>
-      <c r="Z6" s="4">
+      <c r="Z6" s="5">
         <v>4815411515593</v>
       </c>
       <c r="AA6" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AB6" s="3">
+      <c r="AB6" s="4">
         <v>45078</v>
       </c>
-      <c r="AC6" s="5"/>
+      <c r="AC6" s="6"/>
     </row>
     <row r="7" spans="1:29">
       <c r="A7" s="1" t="s">
@@ -2090,7 +2650,7 @@
       <c r="F7" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="G7" s="2" t="s">
         <v>106</v>
       </c>
       <c r="H7" s="1" t="s">
@@ -2120,7 +2680,7 @@
       <c r="P7" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="Q7" s="6" t="s">
+      <c r="Q7" s="7" t="s">
         <v>112</v>
       </c>
       <c r="R7" s="1" t="s">
@@ -2129,7 +2689,7 @@
       <c r="S7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T7" s="6" t="s">
+      <c r="T7" s="7" t="s">
         <v>113</v>
       </c>
       <c r="U7" s="1">
@@ -2144,19 +2704,19 @@
       <c r="X7" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="Y7" s="3">
+      <c r="Y7" s="4">
         <v>35341</v>
       </c>
-      <c r="Z7" s="4">
+      <c r="Z7" s="5">
         <v>2396827590</v>
       </c>
       <c r="AA7" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AB7" s="3">
+      <c r="AB7" s="4">
         <v>44896</v>
       </c>
-      <c r="AC7" s="5"/>
+      <c r="AC7" s="6"/>
     </row>
     <row r="8" spans="1:29">
       <c r="A8" s="1" t="s">
@@ -2165,7 +2725,7 @@
       <c r="B8" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="3" t="s">
         <v>114</v>
       </c>
       <c r="D8" s="1" t="s">
@@ -2177,7 +2737,7 @@
       <c r="F8" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="G8" s="2" t="s">
         <v>118</v>
       </c>
       <c r="H8" s="1" t="s">
@@ -2207,7 +2767,7 @@
       <c r="P8" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="Q8" s="6" t="s">
+      <c r="Q8" s="7" t="s">
         <v>124</v>
       </c>
       <c r="R8" s="1" t="s">
@@ -2216,7 +2776,7 @@
       <c r="S8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T8" s="6" t="s">
+      <c r="T8" s="7" t="s">
         <v>125</v>
       </c>
       <c r="U8" s="1">
@@ -2231,19 +2791,19 @@
       <c r="X8" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="Y8" s="3">
+      <c r="Y8" s="4">
         <v>35776</v>
       </c>
-      <c r="Z8" s="4">
+      <c r="Z8" s="5">
         <v>8253856895</v>
       </c>
       <c r="AA8" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AB8" s="3">
+      <c r="AB8" s="4">
         <v>44287</v>
       </c>
-      <c r="AC8" s="5"/>
+      <c r="AC8" s="6"/>
     </row>
     <row r="9" spans="1:29">
       <c r="A9" s="1" t="s">
@@ -2264,7 +2824,7 @@
       <c r="F9" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="G9" s="7" t="s">
+      <c r="G9" s="2" t="s">
         <v>130</v>
       </c>
       <c r="H9" s="1" t="s">
@@ -2294,7 +2854,7 @@
       <c r="P9" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="Q9" s="6" t="s">
+      <c r="Q9" s="7" t="s">
         <v>136</v>
       </c>
       <c r="R9" s="1" t="s">
@@ -2303,7 +2863,7 @@
       <c r="S9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T9" s="6" t="s">
+      <c r="T9" s="7" t="s">
         <v>137</v>
       </c>
       <c r="U9" s="1">
@@ -2318,19 +2878,19 @@
       <c r="X9" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="Y9" s="3">
+      <c r="Y9" s="4">
         <v>37231</v>
       </c>
-      <c r="Z9" s="4">
+      <c r="Z9" s="5">
         <v>8711373301</v>
       </c>
       <c r="AA9" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AB9" s="3">
+      <c r="AB9" s="4">
         <v>44866</v>
       </c>
-      <c r="AC9" s="5"/>
+      <c r="AC9" s="6"/>
     </row>
     <row r="10" spans="1:29">
       <c r="A10" s="1" t="s">
@@ -2351,7 +2911,7 @@
       <c r="F10" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="G10" s="7" t="s">
+      <c r="G10" s="2" t="s">
         <v>142</v>
       </c>
       <c r="H10" s="1" t="s">
@@ -2381,7 +2941,7 @@
       <c r="P10" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="Q10" s="6" t="s">
+      <c r="Q10" s="7" t="s">
         <v>148</v>
       </c>
       <c r="R10" s="1" t="s">
@@ -2390,7 +2950,7 @@
       <c r="S10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T10" s="6" t="s">
+      <c r="T10" s="7" t="s">
         <v>149</v>
       </c>
       <c r="U10" s="1">
@@ -2405,19 +2965,19 @@
       <c r="X10" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="Y10" s="3">
+      <c r="Y10" s="4">
         <v>35252</v>
       </c>
-      <c r="Z10" s="4">
+      <c r="Z10" s="5">
         <v>4177741263</v>
       </c>
       <c r="AA10" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AB10" s="3">
+      <c r="AB10" s="4">
         <v>44378</v>
       </c>
-      <c r="AC10" s="5"/>
+      <c r="AC10" s="6"/>
     </row>
     <row r="11" spans="1:29">
       <c r="A11" s="1" t="s">
@@ -2438,7 +2998,7 @@
       <c r="F11" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="G11" s="7" t="s">
+      <c r="G11" s="2" t="s">
         <v>154</v>
       </c>
       <c r="H11" s="1" t="s">
@@ -2468,7 +3028,7 @@
       <c r="P11" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="Q11" s="6" t="s">
+      <c r="Q11" s="7" t="s">
         <v>160</v>
       </c>
       <c r="R11" s="1" t="s">
@@ -2477,7 +3037,7 @@
       <c r="S11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T11" s="6" t="s">
+      <c r="T11" s="7" t="s">
         <v>161</v>
       </c>
       <c r="U11" s="1">
@@ -2492,19 +3052,19 @@
       <c r="X11" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="Y11" s="3">
+      <c r="Y11" s="4">
         <v>36557</v>
       </c>
-      <c r="Z11" s="4">
+      <c r="Z11" s="5">
         <v>3313474391</v>
       </c>
       <c r="AA11" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AB11" s="3">
+      <c r="AB11" s="4">
         <v>44986</v>
       </c>
-      <c r="AC11" s="5"/>
+      <c r="AC11" s="6"/>
     </row>
     <row r="12" spans="1:29">
       <c r="A12" s="1" t="s">
@@ -2525,7 +3085,7 @@
       <c r="F12" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="G12" s="7" t="s">
+      <c r="G12" s="2" t="s">
         <v>168</v>
       </c>
       <c r="H12" s="1" t="s">
@@ -2555,7 +3115,7 @@
       <c r="P12" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="Q12" s="6" t="s">
+      <c r="Q12" s="7" t="s">
         <v>174</v>
       </c>
       <c r="R12" s="1" t="s">
@@ -2564,7 +3124,7 @@
       <c r="S12" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T12" s="6" t="s">
+      <c r="T12" s="7" t="s">
         <v>175</v>
       </c>
       <c r="U12" s="1">
@@ -2579,19 +3139,19 @@
       <c r="X12" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="Y12" s="3">
+      <c r="Y12" s="4">
         <v>35170</v>
       </c>
-      <c r="Z12" s="4">
+      <c r="Z12" s="5">
         <v>3780848780</v>
       </c>
       <c r="AA12" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AB12" s="3">
+      <c r="AB12" s="4">
         <v>44743</v>
       </c>
-      <c r="AC12" s="5"/>
+      <c r="AC12" s="6"/>
     </row>
     <row r="13" spans="1:29">
       <c r="A13" s="1" t="s">
@@ -2612,7 +3172,7 @@
       <c r="F13" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="G13" s="7" t="s">
+      <c r="G13" s="2" t="s">
         <v>180</v>
       </c>
       <c r="H13" s="1" t="s">
@@ -2642,7 +3202,7 @@
       <c r="P13" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="Q13" s="6" t="s">
+      <c r="Q13" s="7" t="s">
         <v>187</v>
       </c>
       <c r="R13" s="1" t="s">
@@ -2651,7 +3211,7 @@
       <c r="S13" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T13" s="6" t="s">
+      <c r="T13" s="7" t="s">
         <v>188</v>
       </c>
       <c r="U13" s="1">
@@ -2666,19 +3226,19 @@
       <c r="X13" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="Y13" s="3">
+      <c r="Y13" s="4">
         <v>38353</v>
       </c>
-      <c r="Z13" s="4">
+      <c r="Z13" s="5">
         <v>1040507145</v>
       </c>
       <c r="AA13" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AB13" s="3">
+      <c r="AB13" s="4">
         <v>44927</v>
       </c>
-      <c r="AC13" s="5"/>
+      <c r="AC13" s="6"/>
     </row>
     <row r="14" spans="1:29">
       <c r="A14" s="1" t="s">
@@ -2699,7 +3259,7 @@
       <c r="F14" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="G14" s="7" t="s">
+      <c r="G14" s="2" t="s">
         <v>193</v>
       </c>
       <c r="H14" s="1" t="s">
@@ -2729,7 +3289,7 @@
       <c r="P14" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="Q14" s="6" t="s">
+      <c r="Q14" s="7" t="s">
         <v>200</v>
       </c>
       <c r="R14" s="1" t="s">
@@ -2738,7 +3298,7 @@
       <c r="S14" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T14" s="6" t="s">
+      <c r="T14" s="7" t="s">
         <v>201</v>
       </c>
       <c r="U14" s="1">
@@ -2753,19 +3313,19 @@
       <c r="X14" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="Y14" s="3">
+      <c r="Y14" s="4">
         <v>38079</v>
       </c>
-      <c r="Z14" s="4">
+      <c r="Z14" s="5">
         <v>8722331728</v>
       </c>
       <c r="AA14" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AB14" s="3">
+      <c r="AB14" s="4">
         <v>44927</v>
       </c>
-      <c r="AC14" s="5"/>
+      <c r="AC14" s="6"/>
     </row>
     <row r="15" spans="1:29">
       <c r="A15" s="1" t="s">
@@ -2786,7 +3346,7 @@
       <c r="F15" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="G15" s="7" t="s">
+      <c r="G15" s="2" t="s">
         <v>206</v>
       </c>
       <c r="H15" s="1" t="s">
@@ -2816,7 +3376,7 @@
       <c r="P15" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="Q15" s="6" t="s">
+      <c r="Q15" s="7" t="s">
         <v>212</v>
       </c>
       <c r="R15" s="1" t="s">
@@ -2825,7 +3385,7 @@
       <c r="S15" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T15" s="6" t="s">
+      <c r="T15" s="7" t="s">
         <v>213</v>
       </c>
       <c r="U15" s="1">
@@ -2840,19 +3400,19 @@
       <c r="X15" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="Y15" s="3">
+      <c r="Y15" s="4">
         <v>36356</v>
       </c>
-      <c r="Z15" s="4">
+      <c r="Z15" s="5">
         <v>8265221047</v>
       </c>
       <c r="AA15" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AB15" s="3">
+      <c r="AB15" s="4">
         <v>44835</v>
       </c>
-      <c r="AC15" s="5"/>
+      <c r="AC15" s="6"/>
     </row>
     <row r="16" spans="1:29">
       <c r="A16" s="1" t="s">
@@ -2873,7 +3433,7 @@
       <c r="F16" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="G16" s="7" t="s">
+      <c r="G16" s="2" t="s">
         <v>218</v>
       </c>
       <c r="H16" s="1" t="s">
@@ -2903,7 +3463,7 @@
       <c r="P16" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="Q16" s="6" t="s">
+      <c r="Q16" s="7" t="s">
         <v>224</v>
       </c>
       <c r="R16" s="1" t="s">
@@ -2912,7 +3472,7 @@
       <c r="S16" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T16" s="6" t="s">
+      <c r="T16" s="7" t="s">
         <v>225</v>
       </c>
       <c r="U16" s="1">
@@ -2927,19 +3487,19 @@
       <c r="X16" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="Y16" s="3">
+      <c r="Y16" s="4">
         <v>34090</v>
       </c>
-      <c r="Z16" s="4">
+      <c r="Z16" s="5">
         <v>7803861173</v>
       </c>
       <c r="AA16" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AB16" s="3">
+      <c r="AB16" s="4">
         <v>44927</v>
       </c>
-      <c r="AC16" s="5"/>
+      <c r="AC16" s="6"/>
     </row>
     <row r="17" spans="1:29">
       <c r="A17" s="1" t="s">
@@ -2960,7 +3520,7 @@
       <c r="F17" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="G17" s="7" t="s">
+      <c r="G17" s="2" t="s">
         <v>230</v>
       </c>
       <c r="H17" s="1" t="s">
@@ -2990,7 +3550,7 @@
       <c r="P17" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="Q17" s="6" t="s">
+      <c r="Q17" s="7" t="s">
         <v>236</v>
       </c>
       <c r="R17" s="1" t="s">
@@ -2999,7 +3559,7 @@
       <c r="S17" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T17" s="6" t="s">
+      <c r="T17" s="7" t="s">
         <v>237</v>
       </c>
       <c r="U17" s="1">
@@ -3014,19 +3574,19 @@
       <c r="X17" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="Y17" s="3">
+      <c r="Y17" s="4">
         <v>35286</v>
       </c>
-      <c r="Z17" s="4">
+      <c r="Z17" s="5">
         <v>4810291000800</v>
       </c>
       <c r="AA17" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AB17" s="3">
+      <c r="AB17" s="4">
         <v>43132</v>
       </c>
-      <c r="AC17" s="5"/>
+      <c r="AC17" s="6"/>
     </row>
     <row r="18" spans="1:29">
       <c r="A18" s="1" t="s">
@@ -3047,7 +3607,7 @@
       <c r="F18" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="G18" s="7" t="s">
+      <c r="G18" s="2" t="s">
         <v>242</v>
       </c>
       <c r="H18" s="1" t="s">
@@ -3086,7 +3646,7 @@
       <c r="S18" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T18" s="6" t="s">
+      <c r="T18" s="7" t="s">
         <v>249</v>
       </c>
       <c r="U18" s="1">
@@ -3101,19 +3661,19 @@
       <c r="X18" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="Y18" s="3">
+      <c r="Y18" s="4">
         <v>37289</v>
       </c>
-      <c r="Z18" s="4">
+      <c r="Z18" s="5">
         <v>3308670938</v>
       </c>
       <c r="AA18" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AB18" s="3">
+      <c r="AB18" s="4">
         <v>44835</v>
       </c>
-      <c r="AC18" s="5"/>
+      <c r="AC18" s="6"/>
     </row>
     <row r="19" spans="1:29">
       <c r="A19" s="1" t="s">
@@ -3134,7 +3694,7 @@
       <c r="F19" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="G19" s="7" t="s">
+      <c r="G19" s="2" t="s">
         <v>256</v>
       </c>
       <c r="H19" s="1" t="s">
@@ -3164,7 +3724,7 @@
       <c r="P19" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="Q19" s="6" t="s">
+      <c r="Q19" s="7" t="s">
         <v>263</v>
       </c>
       <c r="R19" s="1" t="s">
@@ -3173,7 +3733,7 @@
       <c r="S19" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T19" s="6" t="s">
+      <c r="T19" s="7" t="s">
         <v>264</v>
       </c>
       <c r="U19" s="1">
@@ -3188,19 +3748,19 @@
       <c r="X19" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="Y19" s="3">
+      <c r="Y19" s="4">
         <v>36382</v>
       </c>
-      <c r="Z19" s="4">
+      <c r="Z19" s="5">
         <v>7804723877</v>
       </c>
       <c r="AA19" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AB19" s="3">
+      <c r="AB19" s="4">
         <v>44896</v>
       </c>
-      <c r="AC19" s="5"/>
+      <c r="AC19" s="6"/>
     </row>
     <row r="20" spans="1:29">
       <c r="A20" s="1" t="s">
@@ -3221,7 +3781,7 @@
       <c r="F20" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="G20" s="7" t="s">
+      <c r="G20" s="2" t="s">
         <v>269</v>
       </c>
       <c r="H20" s="1" t="s">
@@ -3251,7 +3811,7 @@
       <c r="P20" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="Q20" s="6" t="s">
+      <c r="Q20" s="7" t="s">
         <v>275</v>
       </c>
       <c r="R20" s="1" t="s">
@@ -3260,7 +3820,7 @@
       <c r="S20" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T20" s="6" t="s">
+      <c r="T20" s="7" t="s">
         <v>276</v>
       </c>
       <c r="U20" s="1">
@@ -3275,19 +3835,19 @@
       <c r="X20" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="Y20" s="3">
+      <c r="Y20" s="4">
         <v>34856</v>
       </c>
-      <c r="Z20" s="4">
+      <c r="Z20" s="5">
         <v>4825005007400</v>
       </c>
       <c r="AA20" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AB20" s="3">
+      <c r="AB20" s="4">
         <v>43132</v>
       </c>
-      <c r="AC20" s="5"/>
+      <c r="AC20" s="6"/>
     </row>
     <row r="21" spans="1:29">
       <c r="A21" s="1" t="s">
@@ -3308,7 +3868,7 @@
       <c r="F21" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="G21" s="7" t="s">
+      <c r="G21" s="2" t="s">
         <v>281</v>
       </c>
       <c r="H21" s="1" t="s">
@@ -3338,7 +3898,7 @@
       <c r="P21" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="Q21" s="6" t="s">
+      <c r="Q21" s="7" t="s">
         <v>287</v>
       </c>
       <c r="R21" s="1" t="s">
@@ -3347,7 +3907,7 @@
       <c r="S21" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T21" s="6" t="s">
+      <c r="T21" s="7" t="s">
         <v>288</v>
       </c>
       <c r="U21" s="1">
@@ -3362,19 +3922,19 @@
       <c r="X21" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="Y21" s="3">
+      <c r="Y21" s="4">
         <v>36526</v>
       </c>
-      <c r="Z21" s="4">
+      <c r="Z21" s="5">
         <v>4822504037500</v>
       </c>
       <c r="AA21" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AB21" s="3">
+      <c r="AB21" s="4">
         <v>44166</v>
       </c>
-      <c r="AC21" s="5"/>
+      <c r="AC21" s="6"/>
     </row>
     <row r="22" spans="1:29">
       <c r="A22" s="1" t="s">
@@ -3395,7 +3955,7 @@
       <c r="F22" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="G22" s="7" t="s">
+      <c r="G22" s="2" t="s">
         <v>293</v>
       </c>
       <c r="H22" s="1" t="s">
@@ -3434,7 +3994,7 @@
       <c r="S22" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T22" s="6" t="s">
+      <c r="T22" s="7" t="s">
         <v>300</v>
       </c>
       <c r="U22" s="1">
@@ -3449,19 +4009,19 @@
       <c r="X22" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="Y22" s="3">
+      <c r="Y22" s="4">
         <v>31818</v>
       </c>
-      <c r="Z22" s="4">
+      <c r="Z22" s="5">
         <v>4821103670426</v>
       </c>
       <c r="AA22" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AB22" s="3">
+      <c r="AB22" s="4">
         <v>43132</v>
       </c>
-      <c r="AC22" s="5"/>
+      <c r="AC22" s="6"/>
     </row>
     <row r="23" spans="1:29">
       <c r="A23" s="1" t="s">
@@ -3482,7 +4042,7 @@
       <c r="F23" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="G23" s="7" t="s">
+      <c r="G23" s="2" t="s">
         <v>305</v>
       </c>
       <c r="H23" s="1" t="s">
@@ -3512,7 +4072,7 @@
       <c r="P23" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="Q23" s="6" t="s">
+      <c r="Q23" s="7" t="s">
         <v>310</v>
       </c>
       <c r="R23" s="1" t="s">
@@ -3521,7 +4081,7 @@
       <c r="S23" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T23" s="6" t="s">
+      <c r="T23" s="7" t="s">
         <v>311</v>
       </c>
       <c r="U23" s="1">
@@ -3536,19 +4096,19 @@
       <c r="X23" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="Y23" s="3">
+      <c r="Y23" s="4">
         <v>35430</v>
       </c>
-      <c r="Z23" s="4">
+      <c r="Z23" s="5">
         <v>2829707278</v>
       </c>
       <c r="AA23" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AB23" s="3">
+      <c r="AB23" s="4">
         <v>44621</v>
       </c>
-      <c r="AC23" s="5"/>
+      <c r="AC23" s="6"/>
     </row>
     <row r="24" spans="1:29">
       <c r="A24" s="1" t="s">
@@ -3569,7 +4129,7 @@
       <c r="F24" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="G24" s="7" t="s">
+      <c r="G24" s="2" t="s">
         <v>316</v>
       </c>
       <c r="H24" s="1" t="s">
@@ -3599,7 +4159,7 @@
       <c r="P24" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="Q24" s="6" t="s">
+      <c r="Q24" s="7" t="s">
         <v>323</v>
       </c>
       <c r="R24" s="1" t="s">
@@ -3608,7 +4168,7 @@
       <c r="S24" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T24" s="6" t="s">
+      <c r="T24" s="7" t="s">
         <v>324</v>
       </c>
       <c r="U24" s="1">
@@ -3623,19 +4183,19 @@
       <c r="X24" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="Y24" s="3">
+      <c r="Y24" s="4">
         <v>35476</v>
       </c>
-      <c r="Z24" s="4">
+      <c r="Z24" s="5">
         <v>6910287827</v>
       </c>
       <c r="AA24" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AB24" s="3">
+      <c r="AB24" s="4">
         <v>44743</v>
       </c>
-      <c r="AC24" s="5"/>
+      <c r="AC24" s="6"/>
     </row>
     <row r="25" spans="1:29">
       <c r="A25" s="1" t="s">
@@ -3656,7 +4216,7 @@
       <c r="F25" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="G25" s="7" t="s">
+      <c r="G25" s="2" t="s">
         <v>329</v>
       </c>
       <c r="H25" s="1" t="s">
@@ -3686,7 +4246,7 @@
       <c r="P25" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="Q25" s="6" t="s">
+      <c r="Q25" s="7" t="s">
         <v>335</v>
       </c>
       <c r="R25" s="1" t="s">
@@ -3695,7 +4255,7 @@
       <c r="S25" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T25" s="6" t="s">
+      <c r="T25" s="7" t="s">
         <v>336</v>
       </c>
       <c r="U25" s="1">
@@ -3710,19 +4270,19 @@
       <c r="X25" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="Y25" s="3">
+      <c r="Y25" s="4">
         <v>36885</v>
       </c>
-      <c r="Z25" s="4">
+      <c r="Z25" s="5">
         <v>1510907734</v>
       </c>
       <c r="AA25" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AB25" s="3">
+      <c r="AB25" s="4">
         <v>44348</v>
       </c>
-      <c r="AC25" s="5"/>
+      <c r="AC25" s="6"/>
     </row>
     <row r="26" spans="1:29">
       <c r="A26" s="1" t="s">
@@ -3743,7 +4303,7 @@
       <c r="F26" s="1" t="s">
         <v>340</v>
       </c>
-      <c r="G26" s="7" t="s">
+      <c r="G26" s="2" t="s">
         <v>341</v>
       </c>
       <c r="H26" s="1" t="s">
@@ -3773,7 +4333,7 @@
       <c r="P26" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="Q26" s="6" t="s">
+      <c r="Q26" s="7" t="s">
         <v>347</v>
       </c>
       <c r="R26" s="1" t="s">
@@ -3782,7 +4342,7 @@
       <c r="S26" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T26" s="6" t="s">
+      <c r="T26" s="7" t="s">
         <v>348</v>
       </c>
       <c r="U26" s="1">
@@ -3797,19 +4357,19 @@
       <c r="X26" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="Y26" s="3">
+      <c r="Y26" s="4">
         <v>36114</v>
       </c>
-      <c r="Z26" s="4">
+      <c r="Z26" s="5">
         <v>4821110005000</v>
       </c>
       <c r="AA26" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AB26" s="3">
+      <c r="AB26" s="4">
         <v>43709</v>
       </c>
-      <c r="AC26" s="5"/>
+      <c r="AC26" s="6"/>
     </row>
     <row r="27" spans="1:29">
       <c r="A27" s="1" t="s">
@@ -3830,7 +4390,7 @@
       <c r="F27" s="1" t="s">
         <v>352</v>
       </c>
-      <c r="G27" s="7" t="s">
+      <c r="G27" s="2" t="s">
         <v>353</v>
       </c>
       <c r="H27" s="1" t="s">
@@ -3860,7 +4420,7 @@
       <c r="P27" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="Q27" s="6" t="s">
+      <c r="Q27" s="7" t="s">
         <v>359</v>
       </c>
       <c r="R27" s="1" t="s">
@@ -3869,7 +4429,7 @@
       <c r="S27" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T27" s="6" t="s">
+      <c r="T27" s="7" t="s">
         <v>360</v>
       </c>
       <c r="U27" s="1">
@@ -3884,113 +4444,26 @@
       <c r="X27" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="Y27" s="3">
+      <c r="Y27" s="4">
         <v>36318</v>
       </c>
-      <c r="Z27" s="4" t="s">
+      <c r="Z27" s="5" t="s">
         <v>362</v>
       </c>
       <c r="AA27" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AB27" s="3">
+      <c r="AB27" s="4">
         <v>44470</v>
       </c>
-      <c r="AC27" s="5"/>
+      <c r="AC27" s="6"/>
     </row>
-    <row r="28" spans="1:29">
-      <c r="A28" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>366</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>363</v>
-      </c>
-      <c r="E28" s="7" t="s">
-        <v>364</v>
-      </c>
-      <c r="F28" s="7" t="s">
-        <v>367</v>
-      </c>
-      <c r="G28" s="7" t="s">
-        <v>368</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="I28" s="1" t="s">
-        <v>365</v>
-      </c>
-      <c r="J28" s="1" t="s">
-        <v>370</v>
-      </c>
-      <c r="K28" s="1" t="s">
-        <v>371</v>
-      </c>
-      <c r="L28" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="M28" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="N28" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="O28" s="1" t="s">
-        <v>372</v>
-      </c>
-      <c r="P28" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="Q28" s="8" t="s">
-        <v>373</v>
-      </c>
-      <c r="R28" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="S28" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="T28" s="6" t="s">
-        <v>374</v>
-      </c>
-      <c r="U28" s="1">
-        <v>7000</v>
-      </c>
-      <c r="V28" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="W28" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="X28" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="Y28" s="3">
-        <v>36842</v>
-      </c>
-      <c r="Z28" s="4">
-        <v>7800000000</v>
-      </c>
-      <c r="AA28" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="AB28" s="3">
-        <v>44743</v>
-      </c>
-      <c r="AC28" s="5"/>
-    </row>
-    <row r="31" spans="1:29">
-      <c r="E31"/>
+    <row r="30" spans="5:5">
+      <c r="E30"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>